<commit_message>
update GPS points for site 9
</commit_message>
<xml_diff>
--- a/metadata/aquatic-plant-proj-metadata.xlsx
+++ b/metadata/aquatic-plant-proj-metadata.xlsx
@@ -369,7 +369,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -398,6 +398,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,7 +448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,6 +462,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,13 +490,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.7"/>
@@ -1042,6 +1052,7 @@
       <c r="I19" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1076,11 +1087,11 @@
       <c r="A21" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>40.30213</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>-111.65936</v>
+      <c r="B21" s="4" t="n">
+        <v>40.24724</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>-111.67156</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>88</v>
@@ -1105,11 +1116,11 @@
       <c r="A22" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>40.30213</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>-111.65936</v>
+      <c r="B22" s="4" t="n">
+        <v>40.24724</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>-111.67156</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>88</v>
@@ -1134,10 +1145,10 @@
       <c r="A23" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="5" t="n">
         <v>40.24338</v>
       </c>
-      <c r="C23" s="4" t="n">
+      <c r="C23" s="5" t="n">
         <v>-111.67996</v>
       </c>
       <c r="D23" s="0" t="s">
@@ -1163,10 +1174,10 @@
       <c r="A24" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="5" t="n">
         <v>40.24338</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="5" t="n">
         <v>-111.67996</v>
       </c>
       <c r="D24" s="0" t="s">
@@ -1192,10 +1203,10 @@
       <c r="A25" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="5" t="n">
         <v>40.24338</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="5" t="n">
         <v>-111.67996</v>
       </c>
       <c r="D25" s="0" t="s">

</xml_diff>